<commit_message>
Toca Cambiar de Navegador para cumplir que se descargue automaticamente
</commit_message>
<xml_diff>
--- a/fichas_sena.xlsx
+++ b/fichas_sena.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Registro\Desktop\download-report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Download-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD7409F-9AB1-468C-93A9-65F2C997B677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78064D4C-5A3D-4D19-91BE-C32FEE0B35F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00B93854-D0F4-4249-8659-5BBFB82F9AB9}"/>
   </bookViews>
@@ -34,7 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Fichas</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,14 +391,14 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>3267194</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ya hace diferentes Fichas
</commit_message>
<xml_diff>
--- a/fichas_sena.xlsx
+++ b/fichas_sena.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Download-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78064D4C-5A3D-4D19-91BE-C32FEE0B35F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74D0E14-E11D-4768-85B8-AFA403AAFA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00B93854-D0F4-4249-8659-5BBFB82F9AB9}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8EBE44-D464-4F29-8077-97AD01578E29}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +406,11 @@
         <v>2671143</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3183738</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>